<commit_message>
corrigido motor em 0%
</commit_message>
<xml_diff>
--- a/port_map.xlsx
+++ b/port_map.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -859,7 +859,7 @@
   <dimension ref="B2:AY18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AK16" sqref="AK16"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>